<commit_message>
fixed empty cell from database
</commit_message>
<xml_diff>
--- a/TablicaNamirnica.xlsx
+++ b/TablicaNamirnica.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Korisnik\Desktop\FAKULTET 5\1.semestar\Linearna optimizacija\Seminar\Seminar5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Korisnik\Desktop\DietProblem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C4B53B-9480-4D90-BBBC-3A5081C9F5D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3B4820-A9B3-4B54-9F5A-9B8904BD5610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1855,8 +1855,8 @@
   <dimension ref="A1:P226"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A170" sqref="A170"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F88" sqref="F88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -6243,6 +6243,9 @@
       </c>
       <c r="E88">
         <v>1.35</v>
+      </c>
+      <c r="F88">
+        <v>270</v>
       </c>
       <c r="G88">
         <v>6.8</v>

</xml_diff>

<commit_message>
fixed all images and background width
</commit_message>
<xml_diff>
--- a/TablicaNamirnica.xlsx
+++ b/TablicaNamirnica.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Korisnik\Desktop\DietProblem\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3B4820-A9B3-4B54-9F5A-9B8904BD5610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -828,9 +822,6 @@
     <t>https://podravkaiovariations.azureedge.net/56e48a64-498c-11ea-a7bb-5200a71caea1/v/9ed607bc-4c1b-11ea-9bb0-92f307bc0925/450x600-9ed6ed4e-4c1b-11ea-9140-92f307bc0925.png</t>
   </si>
   <si>
-    <t>https://storage.bljesak.info/article/148290/1280x880/mljeveno-meso-tanjur.jpg</t>
-  </si>
-  <si>
     <t>https://images-popusti.njuskalo.hr/data/image/500x705/2507/piko-parizer-pik-vrbovec-400g-plodine-12533717.jpg</t>
   </si>
   <si>
@@ -897,15 +888,9 @@
     <t>https://media.kaufland.com/images/PPIM/AP_Content_1010/std.lang.all/83/30/Asset_818330.jpg</t>
   </si>
   <si>
-    <t>https://hr.cook-and-food.com/images/116/116424/fc98ab1475cb016bae71b8d35fbc3bc2.jpg</t>
-  </si>
-  <si>
     <t>https://womanexpertus.com/wp-content/uploads/2018/05/Ryba-shuka-800x600.jpg</t>
   </si>
   <si>
-    <t>https://storage.bljesak.info/article/15900/1280x880/bjelanjak-zdjela.jpg</t>
-  </si>
-  <si>
     <t>https://aura.ba/wp-content/uploads/2018/01/kosa-jaje.jpeg</t>
   </si>
   <si>
@@ -1005,9 +990,6 @@
     <t>https://2.bp.blogspot.com/-ZALimvswbd8/V5-rUy36nxI/AAAAAAAAVdI/-qc6PmA94TEqqQioaMySraRH0BoplmSbgCPcB/s1600/IMG_5338-blog-zanetti-mascarpone.jpg</t>
   </si>
   <si>
-    <t>https://dukatshop.hr/980-thickbox_default/dukat-tekuci-jogurt-28-mm-330-g.jpg</t>
-  </si>
-  <si>
     <t>https://best-diy-site.com/img/6708541/salat-latuk-virashivanie.jpg</t>
   </si>
   <si>
@@ -1359,9 +1341,6 @@
     <t>https://zdravija.com/wp-content/uploads/2018/08/Maple-Syrup-1.jpeg</t>
   </si>
   <si>
-    <t>https://storage.bljesak.info/article/175377/1280x880/med-med.jpg</t>
-  </si>
-  <si>
     <t>https://raport.ba/wp-content/uploads/2021/02/nutella.jpg</t>
   </si>
   <si>
@@ -1392,9 +1371,6 @@
     <t>https://www.adiva.hr/wp-content/uploads/2019/01/sladoled-760x525.jpg</t>
   </si>
   <si>
-    <t>https://www.travelmagazine.rs/wp-content/uploads/2020/02/background-candy-card-chocolate-chocolates-concept-1567169-pxhere.com_.jpg</t>
-  </si>
-  <si>
     <t>https://www.koestlin.hr/img/products/Koestlin-SlanoTrajno-SaltasSlani-90.png</t>
   </si>
   <si>
@@ -1416,9 +1392,6 @@
     <t>https://d3d173w0vohr0k.cloudfront.net/ba-ba/products/2e/581ed9441945138c495d4eef0f3ce2/corn-standard-425mlv2.png</t>
   </si>
   <si>
-    <t>https://jatrgovac.com/usdocs/kozje-mlijeko.jpg</t>
-  </si>
-  <si>
     <t>https://mimi.ba/wp-content/uploads/2020/12/Kefir-2.8mm-330gr-Meggle.jpg</t>
   </si>
   <si>
@@ -1450,12 +1423,33 @@
   </si>
   <si>
     <t>Klementina</t>
+  </si>
+  <si>
+    <t>https://static.hayat.ba/2019/12/mljeveno-meso-2.jpg</t>
+  </si>
+  <si>
+    <t>https://sasina-kuhinja.com/wp-content/uploads/2020/12/skampi_sasina_kuhinja_recepti.jpg</t>
+  </si>
+  <si>
+    <t>https://i2.wp.com/syl.ru/misc/i/ai/202416/903117.jpg</t>
+  </si>
+  <si>
+    <t>https://znakovi.hgk.hr/wp-content/uploads/2015/11/Vindija_kozje-05-i-02L-za-PR-480x336.jpg</t>
+  </si>
+  <si>
+    <t>https://patrologija.com/wp-content/uploads/2020/07/133924470.jpg</t>
+  </si>
+  <si>
+    <t>https://image.dnevnik.hr/media/images/920x695/Sep2018/61560275-cokolada.jpg</t>
+  </si>
+  <si>
+    <t>https://www.meggle.rs/_products/d342913294726cd5bb40bfa7932e5355.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ _k_n"/>
   </numFmts>
@@ -1550,7 +1544,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperveza" xfId="1" builtinId="8"/>
-    <cellStyle name="Normalno" xfId="0" builtinId="0"/>
+    <cellStyle name="Obično" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1851,34 +1845,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P226"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F88" sqref="F88"/>
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P144" sqref="P144"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.88671875" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="10.44140625" customWidth="1"/>
-    <col min="10" max="10" width="12.109375" customWidth="1"/>
-    <col min="11" max="11" width="12.88671875" customWidth="1"/>
-    <col min="12" max="12" width="13.109375" customWidth="1"/>
-    <col min="13" max="13" width="12.5546875" customWidth="1"/>
-    <col min="14" max="14" width="13.6640625" style="8" customWidth="1"/>
-    <col min="15" max="15" width="25.44140625" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" style="8" customWidth="1"/>
+    <col min="15" max="15" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.6">
+    <row r="1" spans="1:16" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1928,7 +1922,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15.6">
+    <row r="2" spans="1:16" ht="15.75">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1978,7 +1972,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.6">
+    <row r="3" spans="1:16" ht="15.75">
       <c r="A3" t="s">
         <v>247</v>
       </c>
@@ -2028,7 +2022,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15.6">
+    <row r="4" spans="1:16" ht="15.75">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -2078,7 +2072,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="15.6">
+    <row r="5" spans="1:16" ht="15.75">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2128,7 +2122,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15.6">
+    <row r="6" spans="1:16" ht="15.75">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2178,7 +2172,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15.6">
+    <row r="7" spans="1:16" ht="15.75">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2228,7 +2222,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="15.6">
+    <row r="8" spans="1:16" ht="15.75">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -2278,7 +2272,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="15.6">
+    <row r="9" spans="1:16" ht="15.75">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -2328,7 +2322,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15.6">
+    <row r="10" spans="1:16" ht="15.75">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -2378,7 +2372,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="15.6">
+    <row r="11" spans="1:16" ht="15.75">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -2428,7 +2422,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="15.6">
+    <row r="12" spans="1:16" ht="15.75">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -2478,7 +2472,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="15.6">
+    <row r="13" spans="1:16" ht="15.75">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -2528,7 +2522,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="15.6">
+    <row r="14" spans="1:16" ht="15.75">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -2578,7 +2572,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="15.6">
+    <row r="15" spans="1:16" ht="15.75">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -2628,7 +2622,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="15.6">
+    <row r="16" spans="1:16" ht="15.75">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -2678,7 +2672,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="15.6">
+    <row r="17" spans="1:16" ht="15.75">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -2728,7 +2722,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="15.6">
+    <row r="18" spans="1:16" ht="15.75">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -2778,7 +2772,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="15.6">
+    <row r="19" spans="1:16" ht="15.75">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -2828,7 +2822,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="15.6">
+    <row r="20" spans="1:16" ht="15.75">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -2878,7 +2872,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="15.6">
+    <row r="21" spans="1:16" ht="15.75">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -2925,10 +2919,10 @@
         <v>16</v>
       </c>
       <c r="P21" s="5" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="15.6">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="15.75">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -2975,10 +2969,10 @@
         <v>16</v>
       </c>
       <c r="P22" s="5" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="15.6">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="15.75">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -3025,10 +3019,10 @@
         <v>37</v>
       </c>
       <c r="P23" s="5" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" ht="15.6">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="15.75">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -3075,10 +3069,10 @@
         <v>37</v>
       </c>
       <c r="P24" s="5" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" ht="15.6">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="15.75">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -3125,10 +3119,10 @@
         <v>37</v>
       </c>
       <c r="P25" s="5" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" ht="15.6">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="15.75">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -3175,10 +3169,10 @@
         <v>37</v>
       </c>
       <c r="P26" s="5" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" ht="15.6">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="15.75">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -3225,10 +3219,10 @@
         <v>37</v>
       </c>
       <c r="P27" s="5" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" ht="15.6">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="15.75">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -3275,10 +3269,10 @@
         <v>37</v>
       </c>
       <c r="P28" s="5" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" ht="15.6">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="15.75">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -3325,10 +3319,10 @@
         <v>37</v>
       </c>
       <c r="P29" s="5" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" ht="15.6">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="15.75">
       <c r="A30" t="s">
         <v>44</v>
       </c>
@@ -3375,10 +3369,10 @@
         <v>37</v>
       </c>
       <c r="P30" s="5" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" ht="15.6">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="15.75">
       <c r="A31" t="s">
         <v>45</v>
       </c>
@@ -3425,10 +3419,10 @@
         <v>37</v>
       </c>
       <c r="P31" s="5" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" ht="15.6">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="15.75">
       <c r="A32" t="s">
         <v>46</v>
       </c>
@@ -3475,10 +3469,10 @@
         <v>37</v>
       </c>
       <c r="P32" s="5" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" ht="15.6">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="15.75">
       <c r="A33" t="s">
         <v>47</v>
       </c>
@@ -3525,10 +3519,10 @@
         <v>37</v>
       </c>
       <c r="P33" s="5" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" ht="15.6">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="15.75">
       <c r="A34" t="s">
         <v>48</v>
       </c>
@@ -3575,10 +3569,10 @@
         <v>37</v>
       </c>
       <c r="P34" s="5" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" ht="15.6">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="15.75">
       <c r="A35" t="s">
         <v>49</v>
       </c>
@@ -3625,10 +3619,10 @@
         <v>37</v>
       </c>
       <c r="P35" s="5" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" ht="15.6">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" ht="15.75">
       <c r="A36" t="s">
         <v>50</v>
       </c>
@@ -3675,10 +3669,10 @@
         <v>37</v>
       </c>
       <c r="P36" s="5" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" ht="15.6">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="15.75">
       <c r="A37" t="s">
         <v>51</v>
       </c>
@@ -3725,10 +3719,10 @@
         <v>37</v>
       </c>
       <c r="P37" s="5" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" ht="15.6">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" ht="15.75">
       <c r="A38" t="s">
         <v>52</v>
       </c>
@@ -3775,10 +3769,10 @@
         <v>37</v>
       </c>
       <c r="P38" s="5" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" ht="15.6">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" ht="15.75">
       <c r="A39" t="s">
         <v>53</v>
       </c>
@@ -3825,10 +3819,10 @@
         <v>37</v>
       </c>
       <c r="P39" s="5" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" ht="15.6">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" ht="15.75">
       <c r="A40" t="s">
         <v>54</v>
       </c>
@@ -3875,10 +3869,10 @@
         <v>37</v>
       </c>
       <c r="P40" s="5" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" ht="15.6">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" ht="15.75">
       <c r="A41" t="s">
         <v>55</v>
       </c>
@@ -3925,10 +3919,10 @@
         <v>37</v>
       </c>
       <c r="P41" s="5" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" ht="15.6">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" ht="15.75">
       <c r="A42" t="s">
         <v>56</v>
       </c>
@@ -3975,10 +3969,10 @@
         <v>37</v>
       </c>
       <c r="P42" s="5" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" ht="15.6">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" ht="15.75">
       <c r="A43" t="s">
         <v>57</v>
       </c>
@@ -4025,10 +4019,10 @@
         <v>37</v>
       </c>
       <c r="P43" s="5" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" ht="15.6">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" ht="15.75">
       <c r="A44" t="s">
         <v>58</v>
       </c>
@@ -4075,10 +4069,10 @@
         <v>37</v>
       </c>
       <c r="P44" s="5" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" ht="15.6">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" ht="15.75">
       <c r="A45" t="s">
         <v>59</v>
       </c>
@@ -4125,10 +4119,10 @@
         <v>37</v>
       </c>
       <c r="P45" s="5" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" ht="15.6">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" ht="15.75">
       <c r="A46" t="s">
         <v>60</v>
       </c>
@@ -4175,10 +4169,10 @@
         <v>37</v>
       </c>
       <c r="P46" s="5" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" ht="15.6">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" ht="15.75">
       <c r="A47" t="s">
         <v>61</v>
       </c>
@@ -4225,12 +4219,12 @@
         <v>37</v>
       </c>
       <c r="P47" s="5" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" ht="15.6">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" ht="15.75">
       <c r="A48" s="3" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="B48" s="2">
         <v>52</v>
@@ -4275,10 +4269,10 @@
         <v>62</v>
       </c>
       <c r="P48" s="6" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" ht="15.6">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" ht="15.75">
       <c r="A49" s="3" t="s">
         <v>63</v>
       </c>
@@ -4325,10 +4319,10 @@
         <v>62</v>
       </c>
       <c r="P49" s="5" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" ht="15.6">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" ht="15.75">
       <c r="A50" t="s">
         <v>64</v>
       </c>
@@ -4375,10 +4369,10 @@
         <v>62</v>
       </c>
       <c r="P50" s="5" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" ht="15.6">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" ht="15.75">
       <c r="A51" t="s">
         <v>65</v>
       </c>
@@ -4425,10 +4419,10 @@
         <v>62</v>
       </c>
       <c r="P51" s="5" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" ht="15.6">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" ht="15.75">
       <c r="A52" t="s">
         <v>66</v>
       </c>
@@ -4475,10 +4469,10 @@
         <v>62</v>
       </c>
       <c r="P52" s="6" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" ht="15.6">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" ht="15.75">
       <c r="A53" t="s">
         <v>67</v>
       </c>
@@ -4525,10 +4519,10 @@
         <v>62</v>
       </c>
       <c r="P53" s="5" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" ht="15.6">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" ht="15.75">
       <c r="A54" t="s">
         <v>68</v>
       </c>
@@ -4575,10 +4569,10 @@
         <v>62</v>
       </c>
       <c r="P54" s="5" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16" ht="15.6">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" ht="15.75">
       <c r="A55" t="s">
         <v>69</v>
       </c>
@@ -4625,10 +4619,10 @@
         <v>70</v>
       </c>
       <c r="P55" s="5" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" ht="15.6">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" ht="15.75">
       <c r="A56" t="s">
         <v>71</v>
       </c>
@@ -4675,10 +4669,10 @@
         <v>70</v>
       </c>
       <c r="P56" s="5" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16" ht="15.6">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" ht="15.75">
       <c r="A57" t="s">
         <v>72</v>
       </c>
@@ -4725,10 +4719,10 @@
         <v>70</v>
       </c>
       <c r="P57" s="5" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" ht="15.6">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" ht="15.75">
       <c r="A58" t="s">
         <v>73</v>
       </c>
@@ -4775,10 +4769,10 @@
         <v>70</v>
       </c>
       <c r="P58" s="5" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" ht="15.6">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" ht="15.75">
       <c r="A59" t="s">
         <v>74</v>
       </c>
@@ -4825,10 +4819,10 @@
         <v>70</v>
       </c>
       <c r="P59" s="5" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" ht="15.6">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" ht="15.75">
       <c r="A60" t="s">
         <v>75</v>
       </c>
@@ -4875,10 +4869,10 @@
         <v>70</v>
       </c>
       <c r="P60" s="5" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16" ht="15.6">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" ht="15.75">
       <c r="A61" t="s">
         <v>76</v>
       </c>
@@ -4925,10 +4919,10 @@
         <v>70</v>
       </c>
       <c r="P61" s="5" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16" ht="15.6">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" ht="15.75">
       <c r="A62" t="s">
         <v>77</v>
       </c>
@@ -4975,10 +4969,10 @@
         <v>70</v>
       </c>
       <c r="P62" s="5" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" ht="15.6">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" ht="15.75">
       <c r="A63" t="s">
         <v>78</v>
       </c>
@@ -5025,10 +5019,10 @@
         <v>70</v>
       </c>
       <c r="P63" s="5" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="64" spans="1:16" ht="15.6">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" ht="15.75">
       <c r="A64" t="s">
         <v>79</v>
       </c>
@@ -5075,10 +5069,10 @@
         <v>70</v>
       </c>
       <c r="P64" s="5" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="65" spans="1:16" ht="15.6">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" ht="15.75">
       <c r="A65" t="s">
         <v>80</v>
       </c>
@@ -5125,10 +5119,10 @@
         <v>70</v>
       </c>
       <c r="P65" s="5" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="66" spans="1:16" ht="15.6">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" ht="15.75">
       <c r="A66" t="s">
         <v>81</v>
       </c>
@@ -5175,10 +5169,10 @@
         <v>70</v>
       </c>
       <c r="P66" s="5" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="67" spans="1:16" ht="15.6">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" ht="15.75">
       <c r="A67" t="s">
         <v>82</v>
       </c>
@@ -5225,10 +5219,10 @@
         <v>70</v>
       </c>
       <c r="P67" s="5" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="68" spans="1:16" ht="15.6">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" ht="15.75">
       <c r="A68" t="s">
         <v>83</v>
       </c>
@@ -5275,10 +5269,10 @@
         <v>70</v>
       </c>
       <c r="P68" s="5" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" ht="15.6">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" ht="15.75">
       <c r="A69" t="s">
         <v>84</v>
       </c>
@@ -5325,10 +5319,10 @@
         <v>70</v>
       </c>
       <c r="P69" s="5" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="70" spans="1:16" ht="15.6">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" ht="15.75">
       <c r="A70" t="s">
         <v>85</v>
       </c>
@@ -5375,10 +5369,10 @@
         <v>70</v>
       </c>
       <c r="P70" s="5" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="71" spans="1:16" ht="15.6">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" ht="15.75">
       <c r="A71" t="s">
         <v>86</v>
       </c>
@@ -5425,10 +5419,10 @@
         <v>70</v>
       </c>
       <c r="P71" s="5" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="72" spans="1:16" ht="15.6">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" ht="15.75">
       <c r="A72" t="s">
         <v>87</v>
       </c>
@@ -5475,10 +5469,10 @@
         <v>70</v>
       </c>
       <c r="P72" s="5" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="73" spans="1:16" ht="15.6">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" ht="15.75">
       <c r="A73" t="s">
         <v>88</v>
       </c>
@@ -5525,10 +5519,10 @@
         <v>70</v>
       </c>
       <c r="P73" s="5" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="74" spans="1:16" ht="15.6">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" ht="15.75">
       <c r="A74" t="s">
         <v>89</v>
       </c>
@@ -5575,10 +5569,10 @@
         <v>70</v>
       </c>
       <c r="P74" s="5" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="75" spans="1:16" ht="15.6">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" ht="15.75">
       <c r="A75" t="s">
         <v>90</v>
       </c>
@@ -5625,10 +5619,10 @@
         <v>70</v>
       </c>
       <c r="P75" s="5" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="76" spans="1:16" ht="15.6">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" ht="15.75">
       <c r="A76" t="s">
         <v>91</v>
       </c>
@@ -5675,10 +5669,10 @@
         <v>70</v>
       </c>
       <c r="P76" s="5" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="77" spans="1:16" ht="15.6">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" ht="15.75">
       <c r="A77" t="s">
         <v>92</v>
       </c>
@@ -5725,10 +5719,10 @@
         <v>70</v>
       </c>
       <c r="P77" s="5" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="78" spans="1:16" ht="15.6">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" ht="15.75">
       <c r="A78" t="s">
         <v>93</v>
       </c>
@@ -5775,10 +5769,10 @@
         <v>70</v>
       </c>
       <c r="P78" s="5" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="79" spans="1:16" ht="15.6">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" ht="15.75">
       <c r="A79" t="s">
         <v>94</v>
       </c>
@@ -5825,10 +5819,10 @@
         <v>70</v>
       </c>
       <c r="P79" s="5" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="80" spans="1:16" ht="15.6">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" ht="15.75">
       <c r="A80" t="s">
         <v>95</v>
       </c>
@@ -5875,10 +5869,10 @@
         <v>70</v>
       </c>
       <c r="P80" s="5" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="81" spans="1:16" ht="15.6">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" ht="15.75">
       <c r="A81" t="s">
         <v>96</v>
       </c>
@@ -5925,10 +5919,10 @@
         <v>70</v>
       </c>
       <c r="P81" s="5" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="82" spans="1:16" ht="15.6">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" ht="15.75">
       <c r="A82" t="s">
         <v>97</v>
       </c>
@@ -5975,10 +5969,10 @@
         <v>70</v>
       </c>
       <c r="P82" s="5" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="83" spans="1:16" ht="15.6">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" ht="15.75">
       <c r="A83" t="s">
         <v>98</v>
       </c>
@@ -6025,10 +6019,10 @@
         <v>70</v>
       </c>
       <c r="P83" s="5" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="84" spans="1:16" ht="15.6">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" ht="15.75">
       <c r="A84" t="s">
         <v>99</v>
       </c>
@@ -6075,10 +6069,10 @@
         <v>70</v>
       </c>
       <c r="P84" s="6" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="85" spans="1:16" ht="15.6">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" ht="15.75">
       <c r="A85" t="s">
         <v>100</v>
       </c>
@@ -6125,10 +6119,10 @@
         <v>70</v>
       </c>
       <c r="P85" s="5" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="86" spans="1:16" ht="15.6">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" ht="15.75">
       <c r="A86" t="s">
         <v>101</v>
       </c>
@@ -6175,10 +6169,10 @@
         <v>70</v>
       </c>
       <c r="P86" s="5" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="87" spans="1:16" ht="15.6">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" ht="15.75">
       <c r="A87" t="s">
         <v>102</v>
       </c>
@@ -6225,10 +6219,10 @@
         <v>103</v>
       </c>
       <c r="P87" s="5" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="88" spans="1:16" ht="15.6">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" ht="15.75">
       <c r="A88" t="s">
         <v>104</v>
       </c>
@@ -6275,10 +6269,10 @@
         <v>103</v>
       </c>
       <c r="P88" s="5" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="89" spans="1:16" ht="15.6">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" ht="15.75">
       <c r="A89" t="s">
         <v>105</v>
       </c>
@@ -6325,10 +6319,10 @@
         <v>103</v>
       </c>
       <c r="P89" s="5" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="90" spans="1:16" ht="15.6">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" ht="15.75">
       <c r="A90" t="s">
         <v>106</v>
       </c>
@@ -6375,10 +6369,10 @@
         <v>103</v>
       </c>
       <c r="P90" s="5" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="91" spans="1:16" ht="15.6">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" ht="15.75">
       <c r="A91" t="s">
         <v>107</v>
       </c>
@@ -6425,10 +6419,10 @@
         <v>103</v>
       </c>
       <c r="P91" s="5" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="92" spans="1:16" ht="15.6">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" ht="15.75">
       <c r="A92" t="s">
         <v>108</v>
       </c>
@@ -6475,10 +6469,10 @@
         <v>103</v>
       </c>
       <c r="P92" s="5" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="93" spans="1:16" ht="15.6">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16" ht="15.75">
       <c r="A93" t="s">
         <v>109</v>
       </c>
@@ -6525,10 +6519,10 @@
         <v>103</v>
       </c>
       <c r="P93" s="5" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="94" spans="1:16" ht="15.6">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16" ht="15.75">
       <c r="A94" t="s">
         <v>110</v>
       </c>
@@ -6575,10 +6569,10 @@
         <v>103</v>
       </c>
       <c r="P94" s="5" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="95" spans="1:16" ht="15.6">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16" ht="15.75">
       <c r="A95" t="s">
         <v>111</v>
       </c>
@@ -6625,10 +6619,10 @@
         <v>103</v>
       </c>
       <c r="P95" s="5" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="96" spans="1:16" ht="15.6">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16" ht="15.75">
       <c r="A96" t="s">
         <v>112</v>
       </c>
@@ -6675,10 +6669,10 @@
         <v>103</v>
       </c>
       <c r="P96" s="5" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="97" spans="1:16" ht="15.6">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16" ht="15.75">
       <c r="A97" t="s">
         <v>113</v>
       </c>
@@ -6725,10 +6719,10 @@
         <v>103</v>
       </c>
       <c r="P97" s="6" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="98" spans="1:16" ht="15.6">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16" ht="15.75">
       <c r="A98" t="s">
         <v>114</v>
       </c>
@@ -6775,10 +6769,10 @@
         <v>103</v>
       </c>
       <c r="P98" s="5" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="99" spans="1:16" ht="15.6">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" ht="15.75">
       <c r="A99" t="s">
         <v>115</v>
       </c>
@@ -6825,10 +6819,10 @@
         <v>103</v>
       </c>
       <c r="P99" s="5" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="100" spans="1:16" ht="15.6">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16" ht="15.75">
       <c r="A100" t="s">
         <v>116</v>
       </c>
@@ -6875,10 +6869,10 @@
         <v>103</v>
       </c>
       <c r="P100" s="5" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="101" spans="1:16" ht="15.6">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16" ht="15.75">
       <c r="A101" t="s">
         <v>117</v>
       </c>
@@ -6925,10 +6919,10 @@
         <v>103</v>
       </c>
       <c r="P101" s="5" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="102" spans="1:16" ht="15.6">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="102" spans="1:16" ht="15.75">
       <c r="A102" t="s">
         <v>118</v>
       </c>
@@ -6975,10 +6969,10 @@
         <v>103</v>
       </c>
       <c r="P102" s="5" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="103" spans="1:16" ht="15.6">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="103" spans="1:16" ht="15.75">
       <c r="A103" t="s">
         <v>119</v>
       </c>
@@ -7025,10 +7019,10 @@
         <v>103</v>
       </c>
       <c r="P103" s="5" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="104" spans="1:16" ht="15.6">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="104" spans="1:16" ht="15.75">
       <c r="A104" t="s">
         <v>120</v>
       </c>
@@ -7075,10 +7069,10 @@
         <v>103</v>
       </c>
       <c r="P104" s="6" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="105" spans="1:16" ht="15.6">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="105" spans="1:16" ht="15.75">
       <c r="A105" t="s">
         <v>121</v>
       </c>
@@ -7125,10 +7119,10 @@
         <v>103</v>
       </c>
       <c r="P105" s="5" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="106" spans="1:16" ht="15.6">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="106" spans="1:16" ht="15.75">
       <c r="A106" t="s">
         <v>122</v>
       </c>
@@ -7175,10 +7169,10 @@
         <v>103</v>
       </c>
       <c r="P106" s="6" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="107" spans="1:16" ht="15.6">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="107" spans="1:16" ht="15.75">
       <c r="A107" t="s">
         <v>123</v>
       </c>
@@ -7225,10 +7219,10 @@
         <v>103</v>
       </c>
       <c r="P107" s="5" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="108" spans="1:16" ht="15.6">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="108" spans="1:16" ht="15.75">
       <c r="A108" t="s">
         <v>124</v>
       </c>
@@ -7275,10 +7269,10 @@
         <v>103</v>
       </c>
       <c r="P108" s="5" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="109" spans="1:16" ht="15.6">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="109" spans="1:16" ht="15.75">
       <c r="A109" t="s">
         <v>125</v>
       </c>
@@ -7325,10 +7319,10 @@
         <v>103</v>
       </c>
       <c r="P109" s="5" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="110" spans="1:16" ht="15.6">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16" ht="15.75">
       <c r="A110" t="s">
         <v>126</v>
       </c>
@@ -7375,10 +7369,10 @@
         <v>103</v>
       </c>
       <c r="P110" s="5" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="111" spans="1:16" ht="15.6">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="111" spans="1:16" ht="15.75">
       <c r="A111" t="s">
         <v>127</v>
       </c>
@@ -7425,10 +7419,10 @@
         <v>103</v>
       </c>
       <c r="P111" s="5" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="112" spans="1:16" ht="15.6">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16" ht="15.75">
       <c r="A112" t="s">
         <v>128</v>
       </c>
@@ -7475,10 +7469,10 @@
         <v>103</v>
       </c>
       <c r="P112" s="5" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="113" spans="1:16" ht="15.6">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="113" spans="1:16" ht="15.75">
       <c r="A113" t="s">
         <v>129</v>
       </c>
@@ -7525,10 +7519,10 @@
         <v>103</v>
       </c>
       <c r="P113" s="5" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="114" spans="1:16" ht="15.6">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="114" spans="1:16" ht="15.75">
       <c r="A114" t="s">
         <v>130</v>
       </c>
@@ -7575,10 +7569,10 @@
         <v>103</v>
       </c>
       <c r="P114" s="5" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="115" spans="1:16" ht="15.6">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="115" spans="1:16" ht="15.75">
       <c r="A115" t="s">
         <v>131</v>
       </c>
@@ -7625,10 +7619,10 @@
         <v>103</v>
       </c>
       <c r="P115" s="6" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="116" spans="1:16" ht="15.6">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="116" spans="1:16" ht="15.75">
       <c r="A116" t="s">
         <v>132</v>
       </c>
@@ -7675,10 +7669,10 @@
         <v>103</v>
       </c>
       <c r="P116" s="5" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="117" spans="1:16" ht="15.6">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="117" spans="1:16" ht="15.75">
       <c r="A117" t="s">
         <v>133</v>
       </c>
@@ -7725,10 +7719,10 @@
         <v>103</v>
       </c>
       <c r="P117" s="5" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="118" spans="1:16" ht="15.6">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="118" spans="1:16" ht="15.75">
       <c r="A118" t="s">
         <v>134</v>
       </c>
@@ -7775,10 +7769,10 @@
         <v>103</v>
       </c>
       <c r="P118" s="5" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="119" spans="1:16" ht="15.6">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="119" spans="1:16" ht="15.75">
       <c r="A119" t="s">
         <v>135</v>
       </c>
@@ -7825,10 +7819,10 @@
         <v>103</v>
       </c>
       <c r="P119" s="5" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="120" spans="1:16" ht="15.6">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16" ht="15.75">
       <c r="A120" t="s">
         <v>136</v>
       </c>
@@ -7875,10 +7869,10 @@
         <v>103</v>
       </c>
       <c r="P120" s="5" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="121" spans="1:16" ht="15.6">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="121" spans="1:16" ht="15.75">
       <c r="A121" t="s">
         <v>137</v>
       </c>
@@ -7925,10 +7919,10 @@
         <v>103</v>
       </c>
       <c r="P121" s="5" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="122" spans="1:16" ht="15.6">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="122" spans="1:16" ht="15.75">
       <c r="A122" t="s">
         <v>138</v>
       </c>
@@ -7975,10 +7969,10 @@
         <v>103</v>
       </c>
       <c r="P122" s="5" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="123" spans="1:16" ht="15.6">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="123" spans="1:16" ht="15.75">
       <c r="A123" t="s">
         <v>139</v>
       </c>
@@ -8025,10 +8019,10 @@
         <v>103</v>
       </c>
       <c r="P123" s="5" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="124" spans="1:16" ht="15.6">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="124" spans="1:16" ht="15.75">
       <c r="A124" t="s">
         <v>140</v>
       </c>
@@ -8075,10 +8069,10 @@
         <v>103</v>
       </c>
       <c r="P124" s="5" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="125" spans="1:16" ht="15.6">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="125" spans="1:16" ht="15.75">
       <c r="A125" t="s">
         <v>141</v>
       </c>
@@ -8125,10 +8119,10 @@
         <v>142</v>
       </c>
       <c r="P125" s="5" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="126" spans="1:16" ht="15.6">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="126" spans="1:16" ht="15.75">
       <c r="A126" t="s">
         <v>143</v>
       </c>
@@ -8175,10 +8169,10 @@
         <v>142</v>
       </c>
       <c r="P126" s="5" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="127" spans="1:16" ht="15.6">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="127" spans="1:16" ht="15.75">
       <c r="A127" t="s">
         <v>144</v>
       </c>
@@ -8225,10 +8219,10 @@
         <v>142</v>
       </c>
       <c r="P127" s="5" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="128" spans="1:16" ht="15.6">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="128" spans="1:16" ht="15.75">
       <c r="A128" t="s">
         <v>145</v>
       </c>
@@ -8275,10 +8269,10 @@
         <v>142</v>
       </c>
       <c r="P128" s="5" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="129" spans="1:16" ht="15.6">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="129" spans="1:16" ht="15.75">
       <c r="A129" t="s">
         <v>146</v>
       </c>
@@ -8325,10 +8319,10 @@
         <v>142</v>
       </c>
       <c r="P129" s="5" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="130" spans="1:16" ht="15.6">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="130" spans="1:16" ht="15.75">
       <c r="A130" t="s">
         <v>147</v>
       </c>
@@ -8375,10 +8369,10 @@
         <v>142</v>
       </c>
       <c r="P130" s="5" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="131" spans="1:16" ht="15.6">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="131" spans="1:16" ht="15.75">
       <c r="A131" t="s">
         <v>148</v>
       </c>
@@ -8425,10 +8419,10 @@
         <v>142</v>
       </c>
       <c r="P131" s="5" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="132" spans="1:16" ht="15.6">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="132" spans="1:16" ht="15.75">
       <c r="A132" t="s">
         <v>149</v>
       </c>
@@ -8475,10 +8469,10 @@
         <v>142</v>
       </c>
       <c r="P132" s="5" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="133" spans="1:16" ht="15.6">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="133" spans="1:16" ht="15.75">
       <c r="A133" t="s">
         <v>150</v>
       </c>
@@ -8525,10 +8519,10 @@
         <v>142</v>
       </c>
       <c r="P133" s="5" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="134" spans="1:16" ht="15.6">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="134" spans="1:16" ht="15.75">
       <c r="A134" t="s">
         <v>151</v>
       </c>
@@ -8575,10 +8569,10 @@
         <v>142</v>
       </c>
       <c r="P134" s="5" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="135" spans="1:16" ht="15.6">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="135" spans="1:16" ht="15.75">
       <c r="A135" t="s">
         <v>152</v>
       </c>
@@ -8625,10 +8619,10 @@
         <v>142</v>
       </c>
       <c r="P135" s="5" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="136" spans="1:16" ht="15.6">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="136" spans="1:16" ht="15.75">
       <c r="A136" t="s">
         <v>153</v>
       </c>
@@ -8675,10 +8669,10 @@
         <v>142</v>
       </c>
       <c r="P136" s="5" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="137" spans="1:16" ht="15.6">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="137" spans="1:16" ht="15.75">
       <c r="A137" t="s">
         <v>154</v>
       </c>
@@ -8725,10 +8719,10 @@
         <v>142</v>
       </c>
       <c r="P137" s="5" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="138" spans="1:16" ht="15.6">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="138" spans="1:16" ht="15.75">
       <c r="A138" t="s">
         <v>155</v>
       </c>
@@ -8775,10 +8769,10 @@
         <v>142</v>
       </c>
       <c r="P138" s="5" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="139" spans="1:16" ht="15.6">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="139" spans="1:16" ht="15.75">
       <c r="A139" t="s">
         <v>156</v>
       </c>
@@ -8825,10 +8819,10 @@
         <v>142</v>
       </c>
       <c r="P139" s="5" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="140" spans="1:16" ht="15.6">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="140" spans="1:16" ht="15.75">
       <c r="A140" t="s">
         <v>157</v>
       </c>
@@ -8875,10 +8869,10 @@
         <v>142</v>
       </c>
       <c r="P140" s="5" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="141" spans="1:16" ht="15.6">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="141" spans="1:16" ht="15.75">
       <c r="A141" t="s">
         <v>158</v>
       </c>
@@ -8925,10 +8919,10 @@
         <v>142</v>
       </c>
       <c r="P141" s="5" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="142" spans="1:16" ht="15.6">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="142" spans="1:16" ht="15.75">
       <c r="A142" t="s">
         <v>159</v>
       </c>
@@ -8975,10 +8969,10 @@
         <v>142</v>
       </c>
       <c r="P142" s="5" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="143" spans="1:16" ht="15.6">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="143" spans="1:16" ht="15.75">
       <c r="A143" t="s">
         <v>160</v>
       </c>
@@ -9025,10 +9019,10 @@
         <v>142</v>
       </c>
       <c r="P143" s="5" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="144" spans="1:16" ht="15.6">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="144" spans="1:16" ht="15.75">
       <c r="A144" t="s">
         <v>161</v>
       </c>
@@ -9075,10 +9069,10 @@
         <v>142</v>
       </c>
       <c r="P144" s="5" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="145" spans="1:16" ht="15.6">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="145" spans="1:16" ht="15.75">
       <c r="A145" t="s">
         <v>162</v>
       </c>
@@ -9125,10 +9119,10 @@
         <v>142</v>
       </c>
       <c r="P145" s="5" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="146" spans="1:16" ht="15.6">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="146" spans="1:16" ht="15.75">
       <c r="A146" t="s">
         <v>163</v>
       </c>
@@ -9175,10 +9169,10 @@
         <v>142</v>
       </c>
       <c r="P146" s="5" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="147" spans="1:16" ht="15.6">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="147" spans="1:16" ht="15.75">
       <c r="A147" t="s">
         <v>164</v>
       </c>
@@ -9225,10 +9219,10 @@
         <v>142</v>
       </c>
       <c r="P147" s="5" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="148" spans="1:16" ht="15.6">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="148" spans="1:16" ht="15.75">
       <c r="A148" t="s">
         <v>165</v>
       </c>
@@ -9275,10 +9269,10 @@
         <v>142</v>
       </c>
       <c r="P148" s="5" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="149" spans="1:16" ht="15.6">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="149" spans="1:16" ht="15.75">
       <c r="A149" t="s">
         <v>166</v>
       </c>
@@ -9325,10 +9319,10 @@
         <v>142</v>
       </c>
       <c r="P149" s="5" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="150" spans="1:16" ht="15.6">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="150" spans="1:16" ht="15.75">
       <c r="A150" t="s">
         <v>167</v>
       </c>
@@ -9375,10 +9369,10 @@
         <v>142</v>
       </c>
       <c r="P150" s="5" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="151" spans="1:16" ht="15.6">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="151" spans="1:16" ht="15.75">
       <c r="A151" t="s">
         <v>168</v>
       </c>
@@ -9425,10 +9419,10 @@
         <v>142</v>
       </c>
       <c r="P151" s="5" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="152" spans="1:16" ht="15.6">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="152" spans="1:16" ht="15.75">
       <c r="A152" t="s">
         <v>169</v>
       </c>
@@ -9475,10 +9469,10 @@
         <v>142</v>
       </c>
       <c r="P152" s="5" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="153" spans="1:16" ht="15.6">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="153" spans="1:16" ht="15.75">
       <c r="A153" t="s">
         <v>170</v>
       </c>
@@ -9525,10 +9519,10 @@
         <v>142</v>
       </c>
       <c r="P153" s="5" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="154" spans="1:16" ht="15.6">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="154" spans="1:16" ht="15.75">
       <c r="A154" t="s">
         <v>171</v>
       </c>
@@ -9575,10 +9569,10 @@
         <v>142</v>
       </c>
       <c r="P154" s="5" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="155" spans="1:16" ht="15.6">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="155" spans="1:16" ht="15.75">
       <c r="A155" t="s">
         <v>172</v>
       </c>
@@ -9625,10 +9619,10 @@
         <v>173</v>
       </c>
       <c r="P155" s="5" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="156" spans="1:16" ht="15.6">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="156" spans="1:16" ht="15.75">
       <c r="A156" t="s">
         <v>174</v>
       </c>
@@ -9675,10 +9669,10 @@
         <v>173</v>
       </c>
       <c r="P156" s="5" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="157" spans="1:16" ht="15.6">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="157" spans="1:16" ht="15.75">
       <c r="A157" t="s">
         <v>175</v>
       </c>
@@ -9725,10 +9719,10 @@
         <v>173</v>
       </c>
       <c r="P157" s="5" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="158" spans="1:16" ht="15.6">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="158" spans="1:16" ht="15.75">
       <c r="A158" t="s">
         <v>176</v>
       </c>
@@ -9775,10 +9769,10 @@
         <v>173</v>
       </c>
       <c r="P158" s="5" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="159" spans="1:16" ht="15.6">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="159" spans="1:16" ht="15.75">
       <c r="A159" t="s">
         <v>177</v>
       </c>
@@ -9825,10 +9819,10 @@
         <v>173</v>
       </c>
       <c r="P159" s="5" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="160" spans="1:16" ht="15.6">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="160" spans="1:16" ht="15.75">
       <c r="A160" t="s">
         <v>178</v>
       </c>
@@ -9875,10 +9869,10 @@
         <v>173</v>
       </c>
       <c r="P160" s="5" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="161" spans="1:16" ht="15.6">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="161" spans="1:16" ht="15.75">
       <c r="A161" t="s">
         <v>179</v>
       </c>
@@ -9925,10 +9919,10 @@
         <v>173</v>
       </c>
       <c r="P161" s="5" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="162" spans="1:16" ht="15.6">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="162" spans="1:16" ht="15.75">
       <c r="A162" t="s">
         <v>180</v>
       </c>
@@ -9975,10 +9969,10 @@
         <v>173</v>
       </c>
       <c r="P162" s="5" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="163" spans="1:16" ht="15.6">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="163" spans="1:16" ht="15.75">
       <c r="A163" t="s">
         <v>181</v>
       </c>
@@ -10025,10 +10019,10 @@
         <v>173</v>
       </c>
       <c r="P163" s="5" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="164" spans="1:16" ht="15.6">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="164" spans="1:16" ht="15.75">
       <c r="A164" t="s">
         <v>182</v>
       </c>
@@ -10075,10 +10069,10 @@
         <v>173</v>
       </c>
       <c r="P164" s="5" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="165" spans="1:16" ht="15.6">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="165" spans="1:16" ht="15.75">
       <c r="A165" t="s">
         <v>183</v>
       </c>
@@ -10125,10 +10119,10 @@
         <v>173</v>
       </c>
       <c r="P165" s="5" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="166" spans="1:16" ht="15.6">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="166" spans="1:16" ht="15.75">
       <c r="A166" t="s">
         <v>184</v>
       </c>
@@ -10175,10 +10169,10 @@
         <v>173</v>
       </c>
       <c r="P166" s="5" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="167" spans="1:16" ht="15.6">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="167" spans="1:16" ht="15.75">
       <c r="A167" t="s">
         <v>185</v>
       </c>
@@ -10225,10 +10219,10 @@
         <v>173</v>
       </c>
       <c r="P167" s="5" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="168" spans="1:16" ht="15.6">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="168" spans="1:16" ht="15.75">
       <c r="A168" t="s">
         <v>186</v>
       </c>
@@ -10275,10 +10269,10 @@
         <v>173</v>
       </c>
       <c r="P168" s="5" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="169" spans="1:16" ht="15.6">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="169" spans="1:16" ht="15.75">
       <c r="A169" t="s">
         <v>187</v>
       </c>
@@ -10325,12 +10319,12 @@
         <v>173</v>
       </c>
       <c r="P169" s="5" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="170" spans="1:16" ht="15.6">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="170" spans="1:16" ht="15.75">
       <c r="A170" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="B170">
         <v>47</v>
@@ -10375,10 +10369,10 @@
         <v>173</v>
       </c>
       <c r="P170" s="5" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="171" spans="1:16" ht="15.6">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="171" spans="1:16" ht="15.75">
       <c r="A171" t="s">
         <v>188</v>
       </c>
@@ -10425,10 +10419,10 @@
         <v>173</v>
       </c>
       <c r="P171" s="5" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="172" spans="1:16" ht="15.6">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="172" spans="1:16" ht="15.75">
       <c r="A172" t="s">
         <v>189</v>
       </c>
@@ -10475,10 +10469,10 @@
         <v>173</v>
       </c>
       <c r="P172" s="5" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="173" spans="1:16" ht="15.6">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="173" spans="1:16" ht="15.75">
       <c r="A173" t="s">
         <v>190</v>
       </c>
@@ -10525,10 +10519,10 @@
         <v>173</v>
       </c>
       <c r="P173" s="5" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="174" spans="1:16" ht="15.6">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="174" spans="1:16" ht="15.75">
       <c r="A174" t="s">
         <v>191</v>
       </c>
@@ -10575,10 +10569,10 @@
         <v>173</v>
       </c>
       <c r="P174" s="5" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="175" spans="1:16" ht="15.6">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="175" spans="1:16" ht="15.75">
       <c r="A175" t="s">
         <v>192</v>
       </c>
@@ -10625,10 +10619,10 @@
         <v>173</v>
       </c>
       <c r="P175" s="5" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="176" spans="1:16" ht="15.6">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="176" spans="1:16" ht="15.75">
       <c r="A176" t="s">
         <v>193</v>
       </c>
@@ -10675,10 +10669,10 @@
         <v>173</v>
       </c>
       <c r="P176" s="5" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="177" spans="1:16" ht="15.6">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="177" spans="1:16" ht="15.75">
       <c r="A177" t="s">
         <v>194</v>
       </c>
@@ -10725,10 +10719,10 @@
         <v>173</v>
       </c>
       <c r="P177" s="5" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="178" spans="1:16" ht="15.6">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="178" spans="1:16" ht="15.75">
       <c r="A178" t="s">
         <v>195</v>
       </c>
@@ -10775,10 +10769,10 @@
         <v>173</v>
       </c>
       <c r="P178" s="5" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="179" spans="1:16" ht="15.6">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="179" spans="1:16" ht="15.75">
       <c r="A179" t="s">
         <v>196</v>
       </c>
@@ -10825,10 +10819,10 @@
         <v>173</v>
       </c>
       <c r="P179" s="5" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="180" spans="1:16" ht="15.6">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="180" spans="1:16" ht="15.75">
       <c r="A180" t="s">
         <v>197</v>
       </c>
@@ -10875,10 +10869,10 @@
         <v>173</v>
       </c>
       <c r="P180" s="5" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="181" spans="1:16" ht="15.6">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="181" spans="1:16" ht="15.75">
       <c r="A181" t="s">
         <v>198</v>
       </c>
@@ -10925,10 +10919,10 @@
         <v>173</v>
       </c>
       <c r="P181" s="5" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="182" spans="1:16" ht="15.6">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="182" spans="1:16" ht="15.75">
       <c r="A182" t="s">
         <v>199</v>
       </c>
@@ -10975,10 +10969,10 @@
         <v>173</v>
       </c>
       <c r="P182" s="5" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="183" spans="1:16" ht="15.6">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="183" spans="1:16" ht="15.75">
       <c r="A183" t="s">
         <v>200</v>
       </c>
@@ -11025,10 +11019,10 @@
         <v>173</v>
       </c>
       <c r="P183" s="5" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="184" spans="1:16" ht="15.6">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="184" spans="1:16" ht="15.75">
       <c r="A184" t="s">
         <v>201</v>
       </c>
@@ -11075,10 +11069,10 @@
         <v>173</v>
       </c>
       <c r="P184" s="5" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="185" spans="1:16" ht="15.6">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="185" spans="1:16" ht="15.75">
       <c r="A185" t="s">
         <v>202</v>
       </c>
@@ -11125,10 +11119,10 @@
         <v>173</v>
       </c>
       <c r="P185" s="5" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="186" spans="1:16" ht="15.6">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="186" spans="1:16" ht="15.75">
       <c r="A186" t="s">
         <v>203</v>
       </c>
@@ -11175,10 +11169,10 @@
         <v>173</v>
       </c>
       <c r="P186" s="5" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="187" spans="1:16" ht="15.6">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="187" spans="1:16" ht="15.75">
       <c r="A187" t="s">
         <v>204</v>
       </c>
@@ -11225,10 +11219,10 @@
         <v>173</v>
       </c>
       <c r="P187" s="5" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="188" spans="1:16" ht="15.6">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="188" spans="1:16" ht="15.75">
       <c r="A188" t="s">
         <v>205</v>
       </c>
@@ -11275,10 +11269,10 @@
         <v>173</v>
       </c>
       <c r="P188" s="5" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="189" spans="1:16" ht="15.6">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="189" spans="1:16" ht="15.75">
       <c r="A189" t="s">
         <v>206</v>
       </c>
@@ -11325,10 +11319,10 @@
         <v>173</v>
       </c>
       <c r="P189" s="5" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="190" spans="1:16" ht="15.6">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="190" spans="1:16" ht="15.75">
       <c r="A190" t="s">
         <v>207</v>
       </c>
@@ -11375,10 +11369,10 @@
         <v>173</v>
       </c>
       <c r="P190" s="5" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="191" spans="1:16" ht="15.6">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="191" spans="1:16" ht="15.75">
       <c r="A191" t="s">
         <v>208</v>
       </c>
@@ -11425,10 +11419,10 @@
         <v>209</v>
       </c>
       <c r="P191" s="5" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="192" spans="1:16" ht="15.6">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="192" spans="1:16" ht="15.75">
       <c r="A192" t="s">
         <v>210</v>
       </c>
@@ -11475,10 +11469,10 @@
         <v>209</v>
       </c>
       <c r="P192" s="5" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="193" spans="1:16" ht="15.6">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="193" spans="1:16" ht="15.75">
       <c r="A193" t="s">
         <v>211</v>
       </c>
@@ -11525,10 +11519,10 @@
         <v>209</v>
       </c>
       <c r="P193" s="5" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="194" spans="1:16" ht="15.6">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="194" spans="1:16" ht="15.75">
       <c r="A194" t="s">
         <v>212</v>
       </c>
@@ -11575,10 +11569,10 @@
         <v>209</v>
       </c>
       <c r="P194" s="5" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="195" spans="1:16" ht="15.6">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="195" spans="1:16" ht="15.75">
       <c r="A195" t="s">
         <v>213</v>
       </c>
@@ -11625,10 +11619,10 @@
         <v>209</v>
       </c>
       <c r="P195" s="5" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="196" spans="1:16" ht="15.6">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="196" spans="1:16" ht="15.75">
       <c r="A196" t="s">
         <v>214</v>
       </c>
@@ -11675,10 +11669,10 @@
         <v>209</v>
       </c>
       <c r="P196" s="5" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="197" spans="1:16" ht="15.6">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="197" spans="1:16" ht="15.75">
       <c r="A197" t="s">
         <v>215</v>
       </c>
@@ -11725,10 +11719,10 @@
         <v>216</v>
       </c>
       <c r="P197" s="5" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="198" spans="1:16" ht="15.6">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="198" spans="1:16" ht="15.75">
       <c r="A198" t="s">
         <v>217</v>
       </c>
@@ -11775,10 +11769,10 @@
         <v>216</v>
       </c>
       <c r="P198" s="5" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="199" spans="1:16" ht="15.6">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="199" spans="1:16" ht="15.75">
       <c r="A199" t="s">
         <v>218</v>
       </c>
@@ -11825,10 +11819,10 @@
         <v>216</v>
       </c>
       <c r="P199" s="5" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="200" spans="1:16" ht="15.6">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="200" spans="1:16" ht="15.75">
       <c r="A200" t="s">
         <v>219</v>
       </c>
@@ -11875,10 +11869,10 @@
         <v>216</v>
       </c>
       <c r="P200" s="5" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="201" spans="1:16" ht="15.6">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="201" spans="1:16" ht="15.75">
       <c r="A201" t="s">
         <v>220</v>
       </c>
@@ -11925,10 +11919,10 @@
         <v>216</v>
       </c>
       <c r="P201" s="5" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="202" spans="1:16" ht="15.6">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="202" spans="1:16" ht="15.75">
       <c r="A202" t="s">
         <v>221</v>
       </c>
@@ -11975,10 +11969,10 @@
         <v>222</v>
       </c>
       <c r="P202" s="5" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="203" spans="1:16" ht="15.6">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="203" spans="1:16" ht="15.75">
       <c r="A203" t="s">
         <v>223</v>
       </c>
@@ -12025,10 +12019,10 @@
         <v>222</v>
       </c>
       <c r="P203" s="5" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="204" spans="1:16" ht="15.6">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="204" spans="1:16" ht="15.75">
       <c r="A204" t="s">
         <v>224</v>
       </c>
@@ -12075,10 +12069,10 @@
         <v>222</v>
       </c>
       <c r="P204" s="5" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="205" spans="1:16" ht="15.6">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="205" spans="1:16" ht="15.75">
       <c r="A205" t="s">
         <v>225</v>
       </c>
@@ -12125,10 +12119,10 @@
         <v>222</v>
       </c>
       <c r="P205" s="5" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="206" spans="1:16" ht="15.6">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="206" spans="1:16" ht="15.75">
       <c r="A206" t="s">
         <v>226</v>
       </c>
@@ -12175,10 +12169,10 @@
         <v>222</v>
       </c>
       <c r="P206" s="5" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="207" spans="1:16" ht="15.6">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="207" spans="1:16" ht="15.75">
       <c r="A207" t="s">
         <v>227</v>
       </c>
@@ -12225,10 +12219,10 @@
         <v>222</v>
       </c>
       <c r="P207" s="5" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="208" spans="1:16" ht="15.6">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="208" spans="1:16" ht="15.75">
       <c r="A208" t="s">
         <v>228</v>
       </c>
@@ -12275,10 +12269,10 @@
         <v>222</v>
       </c>
       <c r="P208" s="5" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="209" spans="1:16" ht="15.6">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="209" spans="1:16" ht="15.75">
       <c r="A209" t="s">
         <v>229</v>
       </c>
@@ -12325,10 +12319,10 @@
         <v>222</v>
       </c>
       <c r="P209" s="5" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="210" spans="1:16" ht="15.6">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="210" spans="1:16" ht="15.75">
       <c r="A210" t="s">
         <v>230</v>
       </c>
@@ -12375,10 +12369,10 @@
         <v>222</v>
       </c>
       <c r="P210" s="5" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="211" spans="1:16" ht="15.6">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="211" spans="1:16" ht="15.75">
       <c r="A211" t="s">
         <v>231</v>
       </c>
@@ -12425,10 +12419,10 @@
         <v>222</v>
       </c>
       <c r="P211" s="5" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="212" spans="1:16" ht="15.6">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="212" spans="1:16" ht="15.75">
       <c r="A212" t="s">
         <v>232</v>
       </c>
@@ -12475,10 +12469,10 @@
         <v>222</v>
       </c>
       <c r="P212" s="5" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="213" spans="1:16" ht="15.6">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="213" spans="1:16" ht="15.75">
       <c r="A213" t="s">
         <v>233</v>
       </c>
@@ -12525,10 +12519,10 @@
         <v>222</v>
       </c>
       <c r="P213" s="5" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="214" spans="1:16" ht="15.6">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="214" spans="1:16" ht="15.75">
       <c r="A214" t="s">
         <v>234</v>
       </c>
@@ -12575,10 +12569,10 @@
         <v>222</v>
       </c>
       <c r="P214" s="5" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="215" spans="1:16" ht="15.6">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="215" spans="1:16" ht="15.75">
       <c r="A215" t="s">
         <v>235</v>
       </c>
@@ -12625,10 +12619,10 @@
         <v>222</v>
       </c>
       <c r="P215" s="5" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="216" spans="1:16" ht="15.6">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="216" spans="1:16" ht="15.75">
       <c r="A216" t="s">
         <v>236</v>
       </c>
@@ -12675,10 +12669,10 @@
         <v>222</v>
       </c>
       <c r="P216" s="5" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="217" spans="1:16" ht="15.6">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="217" spans="1:16" ht="15.75">
       <c r="A217" t="s">
         <v>237</v>
       </c>
@@ -12725,10 +12719,10 @@
         <v>222</v>
       </c>
       <c r="P217" s="5" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="218" spans="1:16" ht="15.6">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="218" spans="1:16" ht="15.75">
       <c r="A218" t="s">
         <v>238</v>
       </c>
@@ -12775,10 +12769,10 @@
         <v>222</v>
       </c>
       <c r="P218" s="5" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="219" spans="1:16" ht="15.6">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="219" spans="1:16" ht="15.75">
       <c r="A219" t="s">
         <v>239</v>
       </c>
@@ -12825,10 +12819,10 @@
         <v>222</v>
       </c>
       <c r="P219" s="5" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="220" spans="1:16" ht="15.6">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="220" spans="1:16" ht="15.75">
       <c r="A220" t="s">
         <v>240</v>
       </c>
@@ -12875,10 +12869,10 @@
         <v>222</v>
       </c>
       <c r="P220" s="5" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="221" spans="1:16" ht="15.6">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="221" spans="1:16" ht="15.75">
       <c r="A221" t="s">
         <v>241</v>
       </c>
@@ -12925,10 +12919,10 @@
         <v>222</v>
       </c>
       <c r="P221" s="5" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="222" spans="1:16" ht="15.6">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="222" spans="1:16" ht="15.75">
       <c r="A222" t="s">
         <v>242</v>
       </c>
@@ -12975,10 +12969,10 @@
         <v>222</v>
       </c>
       <c r="P222" s="5" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="223" spans="1:16" ht="15.6">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="223" spans="1:16" ht="15.75">
       <c r="A223" t="s">
         <v>243</v>
       </c>
@@ -13025,10 +13019,10 @@
         <v>222</v>
       </c>
       <c r="P223" s="5" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="224" spans="1:16" ht="15.6">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="224" spans="1:16" ht="15.75">
       <c r="A224" t="s">
         <v>244</v>
       </c>
@@ -13075,10 +13069,10 @@
         <v>222</v>
       </c>
       <c r="P224" s="5" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="225" spans="1:16" ht="15.6">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="225" spans="1:16" ht="15.75">
       <c r="A225" t="s">
         <v>245</v>
       </c>
@@ -13125,10 +13119,10 @@
         <v>222</v>
       </c>
       <c r="P225" s="5" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="226" spans="1:16" ht="15.6">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="226" spans="1:16" ht="15.75">
       <c r="A226" t="s">
         <v>246</v>
       </c>
@@ -13175,34 +13169,44 @@
         <v>222</v>
       </c>
       <c r="P226" s="5" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="P21" r:id="rId1"/>
+    <hyperlink ref="P46" r:id="rId2"/>
+    <hyperlink ref="P48" r:id="rId3"/>
+    <hyperlink ref="P73" r:id="rId4"/>
+    <hyperlink ref="P212" r:id="rId5"/>
+    <hyperlink ref="P224" r:id="rId6"/>
+    <hyperlink ref="P86" r:id="rId7"/>
+    <hyperlink ref="P144" r:id="rId8"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>